<commit_message>
Add Mape Leaf and more coins
</commit_message>
<xml_diff>
--- a/precioplata.xlsx
+++ b/precioplata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D705"/>
+  <dimension ref="A1:D713"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15931,6 +15931,182 @@
         </is>
       </c>
     </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Germania</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>1927.2</t>
+        </is>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Fuera de Stock	</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>American Eagle</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>36.01</t>
+        </is>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Disponible  </t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Panda</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>34.73</t>
+        </is>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Disponible  </t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Wedge Tailed</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>1927.2</t>
+        </is>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Agotado Temporalmente	</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Koala</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>229.31</t>
+        </is>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Fuera de Stock	</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Krugerrand</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>28.81</t>
+        </is>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Disponible  </t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Britannia</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>229.31</t>
+        </is>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Fuera de Stock	</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>07/06/2023 23:56</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Filarmonica</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>27.76</t>
+        </is>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		Disponible  </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>